<commit_message>
Fixed typo in group label
</commit_message>
<xml_diff>
--- a/workfiles/examples/Hackathon/FDA STF.xlsx
+++ b/workfiles/examples/Hackathon/FDA STF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDISC\ars\analysis-results-standard\workfiles\examples\Hackathon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BD61B5-4AB0-4894-B9C1-A6956E0A0506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D8B25A-CDB5-429D-9C0D-36BFE3060D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
@@ -789,9 +789,6 @@
     <t>≥ 65</t>
   </si>
   <si>
-    <t>≥ 65 to &lt; 75</t>
-  </si>
-  <si>
     <t>≥ 75</t>
   </si>
   <si>
@@ -1144,6 +1141,9 @@
   </si>
   <si>
     <t>DocumentRef</t>
+  </si>
+  <si>
+    <t>≥ 65 to &lt;75</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
         <v>169</v>
@@ -1672,18 +1672,18 @@
         <v>206</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -1912,7 +1912,7 @@
         <v>Subject</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -1954,7 +1954,7 @@
         <v>Subject</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1966,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
@@ -1996,7 +1996,7 @@
         <v>Subject</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -2008,7 +2008,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G4" t="s">
         <v>33</v>
@@ -2038,7 +2038,7 @@
         <v>Subject</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -2080,7 +2080,7 @@
         <v>Subject</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G6" t="s">
         <v>30</v>
@@ -2122,22 +2122,22 @@
         <v>Subject</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C7" t="s">
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -2149,7 +2149,7 @@
         <v>7</v>
       </c>
       <c r="L7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M7" t="s">
         <v>8</v>
@@ -2164,19 +2164,19 @@
         <v>Subject</v>
       </c>
       <c r="B8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C8" t="s">
         <v>200</v>
       </c>
       <c r="D8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G8" t="s">
         <v>208</v>
@@ -2191,33 +2191,33 @@
         <v>7</v>
       </c>
       <c r="L8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M8" t="s">
         <v>8</v>
       </c>
       <c r="N8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G9" t="s">
         <v>207</v>
@@ -2232,36 +2232,36 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M9" t="s">
         <v>8</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G10" t="s">
-        <v>209</v>
+        <v>327</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2273,13 +2273,13 @@
         <v>7</v>
       </c>
       <c r="L10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M10" t="s">
         <v>8</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
@@ -2288,22 +2288,22 @@
         <v>Subject</v>
       </c>
       <c r="B11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2315,13 +2315,13 @@
         <v>7</v>
       </c>
       <c r="L11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M11" t="s">
         <v>8</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
@@ -2330,7 +2330,7 @@
         <v>Subject</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C12" t="s">
         <v>142</v>
@@ -2342,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G12" t="s">
         <v>58</v>
@@ -2372,7 +2372,7 @@
         <v>Subject</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" t="s">
         <v>142</v>
@@ -2384,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G13" t="s">
         <v>36</v>
@@ -2414,7 +2414,7 @@
         <v>Subject</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
         <v>142</v>
@@ -2426,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G14" t="s">
         <v>59</v>
@@ -2456,7 +2456,7 @@
         <v>Subject</v>
       </c>
       <c r="B15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" t="s">
         <v>142</v>
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G15" t="s">
         <v>37</v>
@@ -2498,7 +2498,7 @@
         <v>Subject</v>
       </c>
       <c r="B16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" t="s">
         <v>142</v>
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G16" t="s">
         <v>38</v>
@@ -2528,10 +2528,10 @@
         <v>35</v>
       </c>
       <c r="M16" t="s">
+        <v>210</v>
+      </c>
+      <c r="N16" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.45">
@@ -2540,7 +2540,7 @@
         <v>Subject</v>
       </c>
       <c r="B17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C17" t="s">
         <v>62</v>
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G17" t="s">
         <v>60</v>
@@ -2582,7 +2582,7 @@
         <v>Subject</v>
       </c>
       <c r="B18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C18" t="s">
         <v>62</v>
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G18" t="s">
         <v>61</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2741,10 +2741,10 @@
         <v>154</v>
       </c>
       <c r="G2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" t="s">
         <v>223</v>
-      </c>
-      <c r="H2" t="s">
-        <v>224</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -2756,12 +2756,12 @@
         <v>40</v>
       </c>
       <c r="Q2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2776,16 +2776,16 @@
         <v>154</v>
       </c>
       <c r="G3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H3" t="s">
         <v>223</v>
-      </c>
-      <c r="H3" t="s">
-        <v>224</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -2797,24 +2797,24 @@
         <v>40</v>
       </c>
       <c r="Q3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R3" t="s">
+        <v>262</v>
+      </c>
+      <c r="S3" t="s">
+        <v>242</v>
+      </c>
+      <c r="T3" t="s">
         <v>263</v>
       </c>
-      <c r="S3" t="s">
-        <v>243</v>
-      </c>
-      <c r="T3" t="s">
-        <v>264</v>
-      </c>
       <c r="U3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2829,10 +2829,10 @@
         <v>154</v>
       </c>
       <c r="G4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" t="s">
         <v>223</v>
-      </c>
-      <c r="H4" t="s">
-        <v>224</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -2844,12 +2844,12 @@
         <v>41</v>
       </c>
       <c r="Q4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2864,22 +2864,22 @@
         <v>154</v>
       </c>
       <c r="G5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H5" t="s">
         <v>223</v>
-      </c>
-      <c r="H5" t="s">
-        <v>224</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -2891,24 +2891,24 @@
         <v>40</v>
       </c>
       <c r="Q5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R5" t="s">
+        <v>262</v>
+      </c>
+      <c r="S5" t="s">
+        <v>241</v>
+      </c>
+      <c r="T5" t="s">
         <v>263</v>
       </c>
-      <c r="S5" t="s">
-        <v>242</v>
-      </c>
-      <c r="T5" t="s">
-        <v>264</v>
-      </c>
       <c r="U5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2923,16 +2923,16 @@
         <v>154</v>
       </c>
       <c r="G6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H6" t="s">
         <v>223</v>
-      </c>
-      <c r="H6" t="s">
-        <v>224</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K6" t="b">
         <v>1</v>
@@ -2944,24 +2944,24 @@
         <v>40</v>
       </c>
       <c r="Q6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R6" t="s">
+        <v>262</v>
+      </c>
+      <c r="S6" t="s">
+        <v>244</v>
+      </c>
+      <c r="T6" t="s">
         <v>263</v>
       </c>
-      <c r="S6" t="s">
-        <v>245</v>
-      </c>
-      <c r="T6" t="s">
-        <v>264</v>
-      </c>
       <c r="U6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2976,16 +2976,16 @@
         <v>154</v>
       </c>
       <c r="G7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H7" t="s">
         <v>223</v>
-      </c>
-      <c r="H7" t="s">
-        <v>224</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
@@ -2997,19 +2997,19 @@
         <v>40</v>
       </c>
       <c r="Q7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R7" t="s">
+        <v>262</v>
+      </c>
+      <c r="S7" t="s">
+        <v>243</v>
+      </c>
+      <c r="T7" t="s">
         <v>263</v>
       </c>
-      <c r="S7" t="s">
-        <v>244</v>
-      </c>
-      <c r="T7" t="s">
-        <v>264</v>
-      </c>
       <c r="U7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2" t="s">
         <v>169</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
         <v>169</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B4" t="s">
         <v>169</v>
@@ -3188,7 +3188,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B5" t="s">
         <v>169</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
         <v>169</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B7" t="s">
         <v>169</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B8" t="s">
         <v>169</v>
@@ -3362,7 +3362,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
         <v>178</v>
@@ -3374,7 +3374,7 @@
         <v>180</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F2" t="s">
         <v>55</v>
@@ -3386,12 +3386,12 @@
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
         <v>105</v>
@@ -3403,7 +3403,7 @@
         <v>107</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F3" t="s">
         <v>55</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B4" t="s">
         <v>105</v>
@@ -3432,7 +3432,7 @@
         <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F4" t="s">
         <v>56</v>
@@ -3444,28 +3444,28 @@
         <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K4" t="s">
         <v>187</v>
       </c>
       <c r="L4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M4" t="s">
         <v>103</v>
       </c>
       <c r="N4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O4" t="s">
         <v>191</v>
       </c>
       <c r="P4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q4" t="s">
         <v>104</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s">
         <v>65</v>
@@ -3485,7 +3485,7 @@
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
@@ -3497,12 +3497,12 @@
         <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
@@ -3514,7 +3514,7 @@
         <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F6" t="s">
         <v>52</v>
@@ -3526,12 +3526,12 @@
         <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
         <v>65</v>
@@ -3543,7 +3543,7 @@
         <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -3555,12 +3555,12 @@
         <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B8" t="s">
         <v>65</v>
@@ -3572,7 +3572,7 @@
         <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F8" t="s">
         <v>53</v>
@@ -3581,15 +3581,15 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9" t="s">
         <v>65</v>
@@ -3601,7 +3601,7 @@
         <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
@@ -3610,10 +3610,10 @@
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3654,10 +3654,10 @@
         <v>157</v>
       </c>
       <c r="B2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" t="s">
         <v>247</v>
-      </c>
-      <c r="C2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -3673,13 +3673,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" t="s">
         <v>322</v>
-      </c>
-      <c r="C4" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
         <v>169</v>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
         <v>169</v>
@@ -3943,7 +3943,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2" s="4" t="str" cm="1">
         <f t="array" ref="B2">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A2,""),"")</f>
@@ -3958,7 +3958,7 @@
         <v>Grouped count for categorical variable</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F2" s="4" t="str" cm="1">
         <f t="array" ref="F2">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E2,"")</f>
@@ -3969,10 +3969,10 @@
         <v>N = XXX</v>
       </c>
       <c r="H2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" t="s">
         <v>224</v>
-      </c>
-      <c r="I2" t="s">
-        <v>225</v>
       </c>
       <c r="J2" s="4" t="str" cm="1">
         <f t="array" ref="J2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I2)*LEN(I2)&gt;0,"")</f>
@@ -3990,13 +3990,13 @@
         <v>86</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="V2" s="6"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B3" s="4" t="str" cm="1">
         <f t="array" ref="B3">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A3,""),"")</f>
@@ -4011,7 +4011,7 @@
         <v>Grouped count for categorical variable</v>
       </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" s="4" t="str" cm="1">
         <f t="array" ref="F3">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E3,"")</f>
@@ -4022,10 +4022,10 @@
         <v>N = XXX</v>
       </c>
       <c r="H3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J3" s="4" t="str" cm="1">
         <f t="array" ref="J3">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I3)*LEN(I3)&gt;0,"")</f>
@@ -4043,13 +4043,13 @@
         <v>84</v>
       </c>
       <c r="U3" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="V3" s="6"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" s="4" t="str" cm="1">
         <f t="array" ref="B4">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A4,""),"")</f>
@@ -4064,7 +4064,7 @@
         <v>Grouped count for categorical variable</v>
       </c>
       <c r="E4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F4" s="4" t="str" cm="1">
         <f t="array" ref="F4">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E4,"")</f>
@@ -4075,10 +4075,10 @@
         <v>N = XXX</v>
       </c>
       <c r="H4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J4" s="4" t="str" cm="1">
         <f t="array" ref="J4">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I4)*LEN(I4)&gt;0,"")</f>
@@ -4096,13 +4096,13 @@
         <v>84</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="V4" s="6"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B5" s="4" t="str" cm="1">
         <f t="array" ref="B5">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A5,""),"")</f>
@@ -4117,7 +4117,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F5" s="4" t="str" cm="1">
         <f t="array" ref="F5">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E5,"")</f>
@@ -4128,20 +4128,20 @@
         <v>n</v>
       </c>
       <c r="H5" t="s">
+        <v>223</v>
+      </c>
+      <c r="I5" t="s">
         <v>224</v>
-      </c>
-      <c r="I5" t="s">
-        <v>225</v>
       </c>
       <c r="J5" s="4" t="str" cm="1">
         <f t="array" ref="J5">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I5)*LEN(I5)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L5" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5" t="s">
         <v>228</v>
-      </c>
-      <c r="M5" t="s">
-        <v>229</v>
       </c>
       <c r="N5" s="4" t="str" cm="1">
         <f t="array" ref="N5">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M5)*LEN(M5)&gt;0,"")</f>
@@ -4161,7 +4161,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" s="4" t="str" cm="1">
         <f t="array" ref="B6">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A6,""),"")</f>
@@ -4176,7 +4176,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F6" s="4" t="str" cm="1">
         <f t="array" ref="F6">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E6,"")</f>
@@ -4187,20 +4187,20 @@
         <v>(%)</v>
       </c>
       <c r="H6" t="s">
+        <v>223</v>
+      </c>
+      <c r="I6" t="s">
         <v>224</v>
-      </c>
-      <c r="I6" t="s">
-        <v>225</v>
       </c>
       <c r="J6" s="4" t="str" cm="1">
         <f t="array" ref="J6">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I6)*LEN(I6)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L6" t="s">
+        <v>227</v>
+      </c>
+      <c r="M6" t="s">
         <v>228</v>
-      </c>
-      <c r="M6" t="s">
-        <v>229</v>
       </c>
       <c r="N6" s="4" t="str" cm="1">
         <f t="array" ref="N6">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M6)*LEN(M6)&gt;0,"")</f>
@@ -4214,13 +4214,13 @@
         <v>38.372100000000003</v>
       </c>
       <c r="U6" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="V6" s="6"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" s="4" t="str" cm="1">
         <f t="array" ref="B7">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A7,""),"")</f>
@@ -4235,7 +4235,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F7" s="4" t="str" cm="1">
         <f t="array" ref="F7">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E7,"")</f>
@@ -4246,20 +4246,20 @@
         <v>n</v>
       </c>
       <c r="H7" t="s">
+        <v>223</v>
+      </c>
+      <c r="I7" t="s">
         <v>224</v>
-      </c>
-      <c r="I7" t="s">
-        <v>225</v>
       </c>
       <c r="J7" s="4" t="str" cm="1">
         <f t="array" ref="J7">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I7)*LEN(I7)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N7" s="4" t="str" cm="1">
         <f t="array" ref="N7">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M7)*LEN(M7)&gt;0,"")</f>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" s="4" t="str" cm="1">
         <f t="array" ref="B8">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A8,""),"")</f>
@@ -4294,7 +4294,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F8" s="4" t="str" cm="1">
         <f t="array" ref="F8">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E8,"")</f>
@@ -4305,20 +4305,20 @@
         <v>(%)</v>
       </c>
       <c r="H8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I8" t="s">
         <v>224</v>
-      </c>
-      <c r="I8" t="s">
-        <v>225</v>
       </c>
       <c r="J8" s="4" t="str" cm="1">
         <f t="array" ref="J8">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I8)*LEN(I8)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N8" s="4" t="str" cm="1">
         <f t="array" ref="N8">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M8)*LEN(M8)&gt;0,"")</f>
@@ -4332,13 +4332,13 @@
         <v>61.627899999999997</v>
       </c>
       <c r="U8" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="V8" s="6"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B9" s="4" t="str" cm="1">
         <f t="array" ref="B9">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A9,""),"")</f>
@@ -4353,7 +4353,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F9" s="4" t="str" cm="1">
         <f t="array" ref="F9">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E9,"")</f>
@@ -4364,20 +4364,20 @@
         <v>n</v>
       </c>
       <c r="H9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J9" s="4" t="str" cm="1">
         <f t="array" ref="J9">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I9)*LEN(I9)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L9" t="s">
+        <v>227</v>
+      </c>
+      <c r="M9" t="s">
         <v>228</v>
-      </c>
-      <c r="M9" t="s">
-        <v>229</v>
       </c>
       <c r="N9" s="4" t="str" cm="1">
         <f t="array" ref="N9">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M9)*LEN(M9)&gt;0,"")</f>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B10" s="4" t="str" cm="1">
         <f t="array" ref="B10">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A10,""),"")</f>
@@ -4412,7 +4412,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F10" s="4" t="str" cm="1">
         <f t="array" ref="F10">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E10,"")</f>
@@ -4423,20 +4423,20 @@
         <v>(%)</v>
       </c>
       <c r="H10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J10" s="4" t="str" cm="1">
         <f t="array" ref="J10">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I10)*LEN(I10)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L10" t="s">
+        <v>227</v>
+      </c>
+      <c r="M10" t="s">
         <v>228</v>
-      </c>
-      <c r="M10" t="s">
-        <v>229</v>
       </c>
       <c r="N10" s="4" t="str" cm="1">
         <f t="array" ref="N10">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M10)*LEN(M10)&gt;0,"")</f>
@@ -4450,13 +4450,13 @@
         <v>40.476199999999999</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="V10" s="6"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B11" s="4" t="str" cm="1">
         <f t="array" ref="B11">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A11,""),"")</f>
@@ -4471,7 +4471,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F11" s="4" t="str" cm="1">
         <f t="array" ref="F11">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E11,"")</f>
@@ -4482,20 +4482,20 @@
         <v>n</v>
       </c>
       <c r="H11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J11" s="4" t="str" cm="1">
         <f t="array" ref="J11">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I11)*LEN(I11)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N11" s="4" t="str" cm="1">
         <f t="array" ref="N11">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M11)*LEN(M11)&gt;0,"")</f>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12" s="4" t="str" cm="1">
         <f t="array" ref="B12">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A12,""),"")</f>
@@ -4530,7 +4530,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F12" s="4" t="str" cm="1">
         <f t="array" ref="F12">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E12,"")</f>
@@ -4541,20 +4541,20 @@
         <v>(%)</v>
       </c>
       <c r="H12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J12" s="4" t="str" cm="1">
         <f t="array" ref="J12">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I12)*LEN(I12)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N12" s="4" t="str" cm="1">
         <f t="array" ref="N12">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M12)*LEN(M12)&gt;0,"")</f>
@@ -4568,13 +4568,13 @@
         <v>59.523800000000001</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="V12" s="6"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13" s="4" t="str" cm="1">
         <f t="array" ref="B13">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A13,""),"")</f>
@@ -4589,7 +4589,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F13" s="4" t="str" cm="1">
         <f t="array" ref="F13">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E13,"")</f>
@@ -4600,20 +4600,20 @@
         <v>n</v>
       </c>
       <c r="H13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J13" s="4" t="str" cm="1">
         <f t="array" ref="J13">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I13)*LEN(I13)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L13" t="s">
+        <v>227</v>
+      </c>
+      <c r="M13" t="s">
         <v>228</v>
-      </c>
-      <c r="M13" t="s">
-        <v>229</v>
       </c>
       <c r="N13" s="4" t="str" cm="1">
         <f t="array" ref="N13">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M13)*LEN(M13)&gt;0,"")</f>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" s="4" t="str" cm="1">
         <f t="array" ref="B14">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A14,""),"")</f>
@@ -4648,7 +4648,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F14" s="4" t="str" cm="1">
         <f t="array" ref="F14">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E14,"")</f>
@@ -4659,20 +4659,20 @@
         <v>(%)</v>
       </c>
       <c r="H14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J14" s="4" t="str" cm="1">
         <f t="array" ref="J14">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I14)*LEN(I14)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L14" t="s">
+        <v>227</v>
+      </c>
+      <c r="M14" t="s">
         <v>228</v>
-      </c>
-      <c r="M14" t="s">
-        <v>229</v>
       </c>
       <c r="N14" s="4" t="str" cm="1">
         <f t="array" ref="N14">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M14)*LEN(M14)&gt;0,"")</f>
@@ -4686,13 +4686,13 @@
         <v>52.381</v>
       </c>
       <c r="U14" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="V14" s="6"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15" s="4" t="str" cm="1">
         <f t="array" ref="B15">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A15,""),"")</f>
@@ -4707,7 +4707,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F15" s="4" t="str" cm="1">
         <f t="array" ref="F15">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E15,"")</f>
@@ -4718,20 +4718,20 @@
         <v>n</v>
       </c>
       <c r="H15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J15" s="4" t="str" cm="1">
         <f t="array" ref="J15">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I15)*LEN(I15)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N15" s="4" t="str" cm="1">
         <f t="array" ref="N15">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M15)*LEN(M15)&gt;0,"")</f>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B16" s="4" t="str" cm="1">
         <f t="array" ref="B16">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A16,""),"")</f>
@@ -4766,7 +4766,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F16" s="4" t="str" cm="1">
         <f t="array" ref="F16">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E16,"")</f>
@@ -4777,20 +4777,20 @@
         <v>(%)</v>
       </c>
       <c r="H16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J16" s="4" t="str" cm="1">
         <f t="array" ref="J16">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I16)*LEN(I16)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N16" s="4" t="str" cm="1">
         <f t="array" ref="N16">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M16)*LEN(M16)&gt;0,"")</f>
@@ -4804,13 +4804,13 @@
         <v>47.619</v>
       </c>
       <c r="U16" s="11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="V16" s="6"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B17" s="4" t="str" cm="1">
         <f t="array" ref="B17">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A17,""),"")</f>
@@ -4825,7 +4825,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F17" s="4" t="str" cm="1">
         <f t="array" ref="F17">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E17,"")</f>
@@ -4836,10 +4836,10 @@
         <v>X.X</v>
       </c>
       <c r="H17" t="s">
+        <v>223</v>
+      </c>
+      <c r="I17" t="s">
         <v>224</v>
-      </c>
-      <c r="I17" t="s">
-        <v>225</v>
       </c>
       <c r="J17" s="4" t="str" cm="1">
         <f t="array" ref="J17">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I17)*LEN(I17)&gt;0,"")</f>
@@ -4863,7 +4863,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B18" s="4" t="str" cm="1">
         <f t="array" ref="B18">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A18,""),"")</f>
@@ -4878,7 +4878,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F18" s="4" t="str" cm="1">
         <f t="array" ref="F18">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E18,"")</f>
@@ -4889,10 +4889,10 @@
         <v>(Y.Y)</v>
       </c>
       <c r="H18" t="s">
+        <v>223</v>
+      </c>
+      <c r="I18" t="s">
         <v>224</v>
-      </c>
-      <c r="I18" t="s">
-        <v>225</v>
       </c>
       <c r="J18" s="4" t="str" cm="1">
         <f t="array" ref="J18">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I18)*LEN(I18)&gt;0,"")</f>
@@ -4910,13 +4910,13 @@
         <v>8.5901999999999994</v>
       </c>
       <c r="U18" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V18" s="6"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B19" s="4" t="str" cm="1">
         <f t="array" ref="B19">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A19,""),"")</f>
@@ -4931,7 +4931,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F19" s="4" t="str" cm="1">
         <f t="array" ref="F19">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E19,"")</f>
@@ -4942,10 +4942,10 @@
         <v>X.X</v>
       </c>
       <c r="H19" t="s">
+        <v>223</v>
+      </c>
+      <c r="I19" t="s">
         <v>224</v>
-      </c>
-      <c r="I19" t="s">
-        <v>225</v>
       </c>
       <c r="J19" s="4" t="str" cm="1">
         <f t="array" ref="J19">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I19)*LEN(I19)&gt;0,"")</f>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B20" s="4" t="str" cm="1">
         <f t="array" ref="B20">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A20,""),"")</f>
@@ -4984,7 +4984,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F20" s="4" t="str" cm="1">
         <f t="array" ref="F20">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E20,"")</f>
@@ -4995,10 +4995,10 @@
         <v>Y.Y</v>
       </c>
       <c r="H20" t="s">
+        <v>223</v>
+      </c>
+      <c r="I20" t="s">
         <v>224</v>
-      </c>
-      <c r="I20" t="s">
-        <v>225</v>
       </c>
       <c r="J20" s="4" t="str" cm="1">
         <f t="array" ref="J20">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I20)*LEN(I20)&gt;0,"")</f>
@@ -5016,13 +5016,13 @@
         <v>52</v>
       </c>
       <c r="U20" s="11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="V20" s="6"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B21" s="4" t="str" cm="1">
         <f t="array" ref="B21">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A21,""),"")</f>
@@ -5037,7 +5037,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F21" s="4" t="str" cm="1">
         <f t="array" ref="F21">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E21,"")</f>
@@ -5048,10 +5048,10 @@
         <v>Z.Z</v>
       </c>
       <c r="H21" t="s">
+        <v>223</v>
+      </c>
+      <c r="I21" t="s">
         <v>224</v>
-      </c>
-      <c r="I21" t="s">
-        <v>225</v>
       </c>
       <c r="J21" s="4" t="str" cm="1">
         <f t="array" ref="J21">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I21)*LEN(I21)&gt;0,"")</f>
@@ -5069,13 +5069,13 @@
         <v>89</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="V21" s="6"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B22" s="4" t="str" cm="1">
         <f t="array" ref="B22">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A22,""),"")</f>
@@ -5090,7 +5090,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F22" s="4" t="str" cm="1">
         <f t="array" ref="F22">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E22,"")</f>
@@ -5101,10 +5101,10 @@
         <v>X.X</v>
       </c>
       <c r="H22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J22" s="4" t="str" cm="1">
         <f t="array" ref="J22">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I22)*LEN(I22)&gt;0,"")</f>
@@ -5128,7 +5128,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B23" s="4" t="str" cm="1">
         <f t="array" ref="B23">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A23,""),"")</f>
@@ -5143,7 +5143,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F23" s="4" t="str" cm="1">
         <f t="array" ref="F23">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E23,"")</f>
@@ -5154,10 +5154,10 @@
         <v>(Y.Y)</v>
       </c>
       <c r="H23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J23" s="4" t="str" cm="1">
         <f t="array" ref="J23">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I23)*LEN(I23)&gt;0,"")</f>
@@ -5175,13 +5175,13 @@
         <v>8.2860999999999994</v>
       </c>
       <c r="U23" s="11" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24" s="4" t="str" cm="1">
         <f t="array" ref="B24">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A24,""),"")</f>
@@ -5196,7 +5196,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F24" s="4" t="str" cm="1">
         <f t="array" ref="F24">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E24,"")</f>
@@ -5207,10 +5207,10 @@
         <v>X.X</v>
       </c>
       <c r="H24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J24" s="4" t="str" cm="1">
         <f t="array" ref="J24">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I24)*LEN(I24)&gt;0,"")</f>
@@ -5234,7 +5234,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B25" s="4" t="str" cm="1">
         <f t="array" ref="B25">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A25,""),"")</f>
@@ -5249,7 +5249,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F25" s="4" t="str" cm="1">
         <f t="array" ref="F25">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E25,"")</f>
@@ -5260,10 +5260,10 @@
         <v>Y.Y</v>
       </c>
       <c r="H25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J25" s="4" t="str" cm="1">
         <f t="array" ref="J25">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I25)*LEN(I25)&gt;0,"")</f>
@@ -5281,13 +5281,13 @@
         <v>51</v>
       </c>
       <c r="U25" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="V25" s="6"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B26" s="4" t="str" cm="1">
         <f t="array" ref="B26">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A26,""),"")</f>
@@ -5302,7 +5302,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F26" s="4" t="str" cm="1">
         <f t="array" ref="F26">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E26,"")</f>
@@ -5313,10 +5313,10 @@
         <v>Z.Z</v>
       </c>
       <c r="H26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J26" s="4" t="str" cm="1">
         <f t="array" ref="J26">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I26)*LEN(I26)&gt;0,"")</f>
@@ -5334,13 +5334,13 @@
         <v>88</v>
       </c>
       <c r="U26" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V26" s="6"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B27" s="4" t="str" cm="1">
         <f t="array" ref="B27">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A27,""),"")</f>
@@ -5355,7 +5355,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F27" s="4" t="str" cm="1">
         <f t="array" ref="F27">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E27,"")</f>
@@ -5366,10 +5366,10 @@
         <v>X.X</v>
       </c>
       <c r="H27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J27" s="4" t="str" cm="1">
         <f t="array" ref="J27">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I27)*LEN(I27)&gt;0,"")</f>
@@ -5393,7 +5393,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B28" s="4" t="str" cm="1">
         <f t="array" ref="B28">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A28,""),"")</f>
@@ -5408,7 +5408,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F28" s="4" t="str" cm="1">
         <f t="array" ref="F28">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E28,"")</f>
@@ -5419,10 +5419,10 @@
         <v>(Y.Y)</v>
       </c>
       <c r="H28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J28" s="4" t="str" cm="1">
         <f t="array" ref="J28">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I28)*LEN(I28)&gt;0,"")</f>
@@ -5440,13 +5440,13 @@
         <v>7.8860999999999999</v>
       </c>
       <c r="U28" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V28" s="6"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B29" s="4" t="str" cm="1">
         <f t="array" ref="B29">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A29,""),"")</f>
@@ -5461,7 +5461,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F29" s="4" t="str" cm="1">
         <f t="array" ref="F29">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E29,"")</f>
@@ -5472,10 +5472,10 @@
         <v>X.X</v>
       </c>
       <c r="H29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J29" s="4" t="str" cm="1">
         <f t="array" ref="J29">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I29)*LEN(I29)&gt;0,"")</f>
@@ -5499,7 +5499,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B30" s="4" t="str" cm="1">
         <f t="array" ref="B30">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A30,""),"")</f>
@@ -5514,7 +5514,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F30" s="4" t="str" cm="1">
         <f t="array" ref="F30">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E30,"")</f>
@@ -5525,10 +5525,10 @@
         <v>Y.Y</v>
       </c>
       <c r="H30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J30" s="4" t="str" cm="1">
         <f t="array" ref="J30">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I30)*LEN(I30)&gt;0,"")</f>
@@ -5546,13 +5546,13 @@
         <v>56</v>
       </c>
       <c r="U30" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V30" s="6"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B31" s="4" t="str" cm="1">
         <f t="array" ref="B31">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A31,""),"")</f>
@@ -5567,7 +5567,7 @@
         <v>Grouped summary of continuous variable</v>
       </c>
       <c r="E31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F31" s="4" t="str" cm="1">
         <f t="array" ref="F31">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E31,"")</f>
@@ -5578,10 +5578,10 @@
         <v>Z.Z</v>
       </c>
       <c r="H31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J31" s="4" t="str" cm="1">
         <f t="array" ref="J31">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I31)*LEN(I31)&gt;0,"")</f>
@@ -5599,13 +5599,13 @@
         <v>88</v>
       </c>
       <c r="U31" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="V31" s="6"/>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B32" s="4" t="str" cm="1">
         <f t="array" ref="B32">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A32,""),"")</f>
@@ -5620,7 +5620,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F32" s="4" t="str" cm="1">
         <f t="array" ref="F32">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E32,"")</f>
@@ -5631,30 +5631,30 @@
         <v>n</v>
       </c>
       <c r="H32" t="s">
+        <v>223</v>
+      </c>
+      <c r="I32" t="s">
         <v>224</v>
-      </c>
-      <c r="I32" t="s">
-        <v>225</v>
       </c>
       <c r="J32" s="4" t="str" cm="1">
         <f t="array" ref="J32">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I32)*LEN(I32)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N32" s="4" t="str" cm="1">
         <f t="array" ref="N32">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M32)*LEN(M32)&gt;0,"")</f>
         <v>&lt; 65</v>
       </c>
       <c r="P32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R32" s="4" t="str" cm="1">
         <f t="array" ref="R32">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q32)*LEN(Q32)&gt;0,"")</f>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B33" s="4" t="str" cm="1">
         <f t="array" ref="B33">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A33,""),"")</f>
@@ -5685,7 +5685,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F33" s="4" t="str" cm="1">
         <f t="array" ref="F33">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E33,"")</f>
@@ -5696,30 +5696,30 @@
         <v>(%)</v>
       </c>
       <c r="H33" t="s">
+        <v>223</v>
+      </c>
+      <c r="I33" t="s">
         <v>224</v>
-      </c>
-      <c r="I33" t="s">
-        <v>225</v>
       </c>
       <c r="J33" s="4" t="str" cm="1">
         <f t="array" ref="J33">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I33)*LEN(I33)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L33" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N33" s="4" t="str" cm="1">
         <f t="array" ref="N33">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M33)*LEN(M33)&gt;0,"")</f>
         <v>&lt; 65</v>
       </c>
       <c r="P33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R33" s="4" t="str" cm="1">
         <f t="array" ref="R33">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q33)*LEN(Q33)&gt;0,"")</f>
@@ -5729,13 +5729,13 @@
         <v>16.2791</v>
       </c>
       <c r="U33" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="V33" s="6"/>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B34" s="4" t="str" cm="1">
         <f t="array" ref="B34">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A34,""),"")</f>
@@ -5750,7 +5750,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E34" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F34" s="4" t="str" cm="1">
         <f t="array" ref="F34">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E34,"")</f>
@@ -5761,34 +5761,34 @@
         <v>n</v>
       </c>
       <c r="H34" t="s">
+        <v>223</v>
+      </c>
+      <c r="I34" t="s">
         <v>224</v>
-      </c>
-      <c r="I34" t="s">
-        <v>225</v>
       </c>
       <c r="J34" s="4" t="str" cm="1">
         <f t="array" ref="J34">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I34)*LEN(I34)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N34" s="4" t="str" cm="1">
         <f t="array" ref="N34">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M34)*LEN(M34)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R34" s="4" t="str" cm="1">
         <f t="array" ref="R34">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q34)*LEN(Q34)&gt;0,"")</f>
-        <v>≥ 65 to &lt; 75</v>
+        <v>≥ 65 to &lt;75</v>
       </c>
       <c r="T34">
         <v>24</v>
@@ -5800,7 +5800,7 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B35" s="4" t="str" cm="1">
         <f t="array" ref="B35">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A35,""),"")</f>
@@ -5815,7 +5815,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E35" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F35" s="4" t="str" cm="1">
         <f t="array" ref="F35">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E35,"")</f>
@@ -5826,46 +5826,46 @@
         <v>(%)</v>
       </c>
       <c r="H35" t="s">
+        <v>223</v>
+      </c>
+      <c r="I35" t="s">
         <v>224</v>
-      </c>
-      <c r="I35" t="s">
-        <v>225</v>
       </c>
       <c r="J35" s="4" t="str" cm="1">
         <f t="array" ref="J35">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I35)*LEN(I35)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N35" s="4" t="str" cm="1">
         <f t="array" ref="N35">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M35)*LEN(M35)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R35" s="4" t="str" cm="1">
         <f t="array" ref="R35">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q35)*LEN(Q35)&gt;0,"")</f>
-        <v>≥ 65 to &lt; 75</v>
+        <v>≥ 65 to &lt;75</v>
       </c>
       <c r="T35">
         <v>27.907</v>
       </c>
       <c r="U35" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="V35" s="6"/>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B36" s="4" t="str" cm="1">
         <f t="array" ref="B36">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A36,""),"")</f>
@@ -5880,7 +5880,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F36" s="4" t="str" cm="1">
         <f t="array" ref="F36">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E36,"")</f>
@@ -5891,30 +5891,30 @@
         <v>n</v>
       </c>
       <c r="H36" t="s">
+        <v>223</v>
+      </c>
+      <c r="I36" t="s">
         <v>224</v>
-      </c>
-      <c r="I36" t="s">
-        <v>225</v>
       </c>
       <c r="J36" s="4" t="str" cm="1">
         <f t="array" ref="J36">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I36)*LEN(I36)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N36" s="4" t="str" cm="1">
         <f t="array" ref="N36">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M36)*LEN(M36)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R36" s="4" t="str" cm="1">
         <f t="array" ref="R36">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q36)*LEN(Q36)&gt;0,"")</f>
@@ -5930,7 +5930,7 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B37" s="4" t="str" cm="1">
         <f t="array" ref="B37">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A37,""),"")</f>
@@ -5945,7 +5945,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F37" s="4" t="str" cm="1">
         <f t="array" ref="F37">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E37,"")</f>
@@ -5956,30 +5956,30 @@
         <v>(%)</v>
       </c>
       <c r="H37" t="s">
+        <v>223</v>
+      </c>
+      <c r="I37" t="s">
         <v>224</v>
-      </c>
-      <c r="I37" t="s">
-        <v>225</v>
       </c>
       <c r="J37" s="4" t="str" cm="1">
         <f t="array" ref="J37">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I37)*LEN(I37)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N37" s="4" t="str" cm="1">
         <f t="array" ref="N37">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M37)*LEN(M37)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R37" s="4" t="str" cm="1">
         <f t="array" ref="R37">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q37)*LEN(Q37)&gt;0,"")</f>
@@ -5989,13 +5989,13 @@
         <v>55.814</v>
       </c>
       <c r="U37" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="V37" s="6"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B38" s="4" t="str" cm="1">
         <f t="array" ref="B38">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A38,""),"")</f>
@@ -6010,7 +6010,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F38" s="4" t="str" cm="1">
         <f t="array" ref="F38">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E38,"")</f>
@@ -6021,30 +6021,30 @@
         <v>n</v>
       </c>
       <c r="H38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J38" s="4" t="str" cm="1">
         <f t="array" ref="J38">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I38)*LEN(I38)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N38" s="4" t="str" cm="1">
         <f t="array" ref="N38">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M38)*LEN(M38)&gt;0,"")</f>
         <v>&lt; 65</v>
       </c>
       <c r="P38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R38" s="4" t="str" cm="1">
         <f t="array" ref="R38">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q38)*LEN(Q38)&gt;0,"")</f>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B39" s="4" t="str" cm="1">
         <f t="array" ref="B39">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A39,""),"")</f>
@@ -6075,7 +6075,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E39" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F39" s="4" t="str" cm="1">
         <f t="array" ref="F39">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E39,"")</f>
@@ -6086,30 +6086,30 @@
         <v>(%)</v>
       </c>
       <c r="H39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J39" s="4" t="str" cm="1">
         <f t="array" ref="J39">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I39)*LEN(I39)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N39" s="4" t="str" cm="1">
         <f t="array" ref="N39">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M39)*LEN(M39)&gt;0,"")</f>
         <v>&lt; 65</v>
       </c>
       <c r="P39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R39" s="4" t="str" cm="1">
         <f t="array" ref="R39">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q39)*LEN(Q39)&gt;0,"")</f>
@@ -6119,13 +6119,13 @@
         <v>9.5237999999999996</v>
       </c>
       <c r="U39" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="V39" s="6"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B40" s="4" t="str" cm="1">
         <f t="array" ref="B40">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A40,""),"")</f>
@@ -6140,7 +6140,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F40" s="4" t="str" cm="1">
         <f t="array" ref="F40">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E40,"")</f>
@@ -6151,34 +6151,34 @@
         <v>n</v>
       </c>
       <c r="H40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J40" s="4" t="str" cm="1">
         <f t="array" ref="J40">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I40)*LEN(I40)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N40" s="4" t="str" cm="1">
         <f t="array" ref="N40">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M40)*LEN(M40)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P40" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R40" s="4" t="str" cm="1">
         <f t="array" ref="R40">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q40)*LEN(Q40)&gt;0,"")</f>
-        <v>≥ 65 to &lt; 75</v>
+        <v>≥ 65 to &lt;75</v>
       </c>
       <c r="T40">
         <v>23</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B41" s="4" t="str" cm="1">
         <f t="array" ref="B41">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A41,""),"")</f>
@@ -6205,7 +6205,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E41" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F41" s="4" t="str" cm="1">
         <f t="array" ref="F41">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E41,"")</f>
@@ -6216,46 +6216,46 @@
         <v>(%)</v>
       </c>
       <c r="H41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J41" s="4" t="str" cm="1">
         <f t="array" ref="J41">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I41)*LEN(I41)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M41" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N41" s="4" t="str" cm="1">
         <f t="array" ref="N41">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M41)*LEN(M41)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R41" s="4" t="str" cm="1">
         <f t="array" ref="R41">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q41)*LEN(Q41)&gt;0,"")</f>
-        <v>≥ 65 to &lt; 75</v>
+        <v>≥ 65 to &lt;75</v>
       </c>
       <c r="T41">
         <v>27.381</v>
       </c>
       <c r="U41" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="V41" s="6"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B42" s="4" t="str" cm="1">
         <f t="array" ref="B42">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A42,""),"")</f>
@@ -6270,7 +6270,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F42" s="4" t="str" cm="1">
         <f t="array" ref="F42">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E42,"")</f>
@@ -6281,30 +6281,30 @@
         <v>n</v>
       </c>
       <c r="H42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J42" s="4" t="str" cm="1">
         <f t="array" ref="J42">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I42)*LEN(I42)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N42" s="4" t="str" cm="1">
         <f t="array" ref="N42">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M42)*LEN(M42)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R42" s="4" t="str" cm="1">
         <f t="array" ref="R42">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q42)*LEN(Q42)&gt;0,"")</f>
@@ -6320,7 +6320,7 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B43" s="4" t="str" cm="1">
         <f t="array" ref="B43">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A43,""),"")</f>
@@ -6335,7 +6335,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F43" s="4" t="str" cm="1">
         <f t="array" ref="F43">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E43,"")</f>
@@ -6346,30 +6346,30 @@
         <v>(%)</v>
       </c>
       <c r="H43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J43" s="4" t="str" cm="1">
         <f t="array" ref="J43">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I43)*LEN(I43)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N43" s="4" t="str" cm="1">
         <f t="array" ref="N43">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M43)*LEN(M43)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R43" s="4" t="str" cm="1">
         <f t="array" ref="R43">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q43)*LEN(Q43)&gt;0,"")</f>
@@ -6379,13 +6379,13 @@
         <v>63.095199999999998</v>
       </c>
       <c r="U43" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="V43" s="6"/>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B44" s="4" t="str" cm="1">
         <f t="array" ref="B44">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A44,""),"")</f>
@@ -6400,7 +6400,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E44" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F44" s="4" t="str" cm="1">
         <f t="array" ref="F44">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E44,"")</f>
@@ -6411,30 +6411,30 @@
         <v>n</v>
       </c>
       <c r="H44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I44" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J44" s="4" t="str" cm="1">
         <f t="array" ref="J44">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I44)*LEN(I44)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L44" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N44" s="4" t="str" cm="1">
         <f t="array" ref="N44">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M44)*LEN(M44)&gt;0,"")</f>
         <v>&lt; 65</v>
       </c>
       <c r="P44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q44" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R44" s="4" t="str" cm="1">
         <f t="array" ref="R44">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q44)*LEN(Q44)&gt;0,"")</f>
@@ -6450,7 +6450,7 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B45" s="4" t="str" cm="1">
         <f t="array" ref="B45">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A45,""),"")</f>
@@ -6465,7 +6465,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F45" s="4" t="str" cm="1">
         <f t="array" ref="F45">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E45,"")</f>
@@ -6476,30 +6476,30 @@
         <v>(%)</v>
       </c>
       <c r="H45" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J45" s="4" t="str" cm="1">
         <f t="array" ref="J45">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I45)*LEN(I45)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L45" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N45" s="4" t="str" cm="1">
         <f t="array" ref="N45">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M45)*LEN(M45)&gt;0,"")</f>
         <v>&lt; 65</v>
       </c>
       <c r="P45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R45" s="4" t="str" cm="1">
         <f t="array" ref="R45">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q45)*LEN(Q45)&gt;0,"")</f>
@@ -6509,13 +6509,13 @@
         <v>13.0952</v>
       </c>
       <c r="U45" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="V45" s="6"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B46" s="4" t="str" cm="1">
         <f t="array" ref="B46">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A46,""),"")</f>
@@ -6530,7 +6530,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E46" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F46" s="4" t="str" cm="1">
         <f t="array" ref="F46">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E46,"")</f>
@@ -6541,34 +6541,34 @@
         <v>n</v>
       </c>
       <c r="H46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J46" s="4" t="str" cm="1">
         <f t="array" ref="J46">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I46)*LEN(I46)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N46" s="4" t="str" cm="1">
         <f t="array" ref="N46">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M46)*LEN(M46)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R46" s="4" t="str" cm="1">
         <f t="array" ref="R46">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q46)*LEN(Q46)&gt;0,"")</f>
-        <v>≥ 65 to &lt; 75</v>
+        <v>≥ 65 to &lt;75</v>
       </c>
       <c r="T46">
         <v>25</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B47" s="4" t="str" cm="1">
         <f t="array" ref="B47">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A47,""),"")</f>
@@ -6595,7 +6595,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E47" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F47" s="4" t="str" cm="1">
         <f t="array" ref="F47">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E47,"")</f>
@@ -6606,46 +6606,46 @@
         <v>(%)</v>
       </c>
       <c r="H47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J47" s="4" t="str" cm="1">
         <f t="array" ref="J47">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I47)*LEN(I47)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N47" s="4" t="str" cm="1">
         <f t="array" ref="N47">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M47)*LEN(M47)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R47" s="4" t="str" cm="1">
         <f t="array" ref="R47">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q47)*LEN(Q47)&gt;0,"")</f>
-        <v>≥ 65 to &lt; 75</v>
+        <v>≥ 65 to &lt;75</v>
       </c>
       <c r="T47">
         <v>29.761900000000001</v>
       </c>
       <c r="U47" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="V47" s="6"/>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B48" s="4" t="str" cm="1">
         <f t="array" ref="B48">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A48,""),"")</f>
@@ -6660,7 +6660,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F48" s="4" t="str" cm="1">
         <f t="array" ref="F48">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E48,"")</f>
@@ -6671,30 +6671,30 @@
         <v>n</v>
       </c>
       <c r="H48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J48" s="4" t="str" cm="1">
         <f t="array" ref="J48">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I48)*LEN(I48)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N48" s="4" t="str" cm="1">
         <f t="array" ref="N48">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M48)*LEN(M48)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R48" s="4" t="str" cm="1">
         <f t="array" ref="R48">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q48)*LEN(Q48)&gt;0,"")</f>
@@ -6710,7 +6710,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B49" s="4" t="str" cm="1">
         <f t="array" ref="B49">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A49,""),"")</f>
@@ -6725,7 +6725,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F49" s="4" t="str" cm="1">
         <f t="array" ref="F49">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E49,"")</f>
@@ -6736,30 +6736,30 @@
         <v>(%)</v>
       </c>
       <c r="H49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J49" s="4" t="str" cm="1">
         <f t="array" ref="J49">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I49)*LEN(I49)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N49" s="4" t="str" cm="1">
         <f t="array" ref="N49">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M49)*LEN(M49)&gt;0,"")</f>
         <v>≥ 65</v>
       </c>
       <c r="P49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Q49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R49" s="4" t="str" cm="1">
         <f t="array" ref="R49">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!Q49)*LEN(Q49)&gt;0,"")</f>
@@ -6769,13 +6769,13 @@
         <v>57.142899999999997</v>
       </c>
       <c r="U49" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V49" s="6"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B50" s="4" t="str" cm="1">
         <f t="array" ref="B50">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A50,""),"")</f>
@@ -6790,7 +6790,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F50" s="4" t="str" cm="1">
         <f t="array" ref="F50">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E50,"")</f>
@@ -6801,20 +6801,20 @@
         <v>n</v>
       </c>
       <c r="H50" t="s">
+        <v>223</v>
+      </c>
+      <c r="I50" t="s">
         <v>224</v>
-      </c>
-      <c r="I50" t="s">
-        <v>225</v>
       </c>
       <c r="J50" s="4" t="str" cm="1">
         <f t="array" ref="J50">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I50)*LEN(I50)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N50" s="4" t="str" cm="1">
         <f t="array" ref="N50">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M50)*LEN(M50)&gt;0,"")</f>
@@ -6834,7 +6834,7 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B51" s="4" t="str" cm="1">
         <f t="array" ref="B51">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A51,""),"")</f>
@@ -6849,7 +6849,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E51" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F51" s="4" t="str" cm="1">
         <f t="array" ref="F51">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E51,"")</f>
@@ -6860,20 +6860,20 @@
         <v>(%)</v>
       </c>
       <c r="H51" t="s">
+        <v>223</v>
+      </c>
+      <c r="I51" t="s">
         <v>224</v>
-      </c>
-      <c r="I51" t="s">
-        <v>225</v>
       </c>
       <c r="J51" s="4" t="str" cm="1">
         <f t="array" ref="J51">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I51)*LEN(I51)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N51" s="4" t="str" cm="1">
         <f t="array" ref="N51">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M51)*LEN(M51)&gt;0,"")</f>
@@ -6887,13 +6887,13 @@
         <v>9.3023000000000007</v>
       </c>
       <c r="U51" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="V51" s="6"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B52" s="4" t="str" cm="1">
         <f t="array" ref="B52">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A52,""),"")</f>
@@ -6908,7 +6908,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F52" s="4" t="str" cm="1">
         <f t="array" ref="F52">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E52,"")</f>
@@ -6919,20 +6919,20 @@
         <v>n</v>
       </c>
       <c r="H52" t="s">
+        <v>223</v>
+      </c>
+      <c r="I52" t="s">
         <v>224</v>
-      </c>
-      <c r="I52" t="s">
-        <v>225</v>
       </c>
       <c r="J52" s="4" t="str" cm="1">
         <f t="array" ref="J52">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I52)*LEN(I52)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M52" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N52" s="4" t="str" cm="1">
         <f t="array" ref="N52">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M52)*LEN(M52)&gt;0,"")</f>
@@ -6952,7 +6952,7 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B53" s="4" t="str" cm="1">
         <f t="array" ref="B53">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A53,""),"")</f>
@@ -6967,7 +6967,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E53" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F53" s="4" t="str" cm="1">
         <f t="array" ref="F53">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E53,"")</f>
@@ -6978,20 +6978,20 @@
         <v>(%)</v>
       </c>
       <c r="H53" t="s">
+        <v>223</v>
+      </c>
+      <c r="I53" t="s">
         <v>224</v>
-      </c>
-      <c r="I53" t="s">
-        <v>225</v>
       </c>
       <c r="J53" s="4" t="str" cm="1">
         <f t="array" ref="J53">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I53)*LEN(I53)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N53" s="4" t="str" cm="1">
         <f t="array" ref="N53">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M53)*LEN(M53)&gt;0,"")</f>
@@ -7005,13 +7005,13 @@
         <v>90.697699999999998</v>
       </c>
       <c r="U53" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="V53" s="6"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B54" s="4" t="str" cm="1">
         <f t="array" ref="B54">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A54,""),"")</f>
@@ -7026,7 +7026,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E54" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F54" s="4" t="str" cm="1">
         <f t="array" ref="F54">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E54,"")</f>
@@ -7037,20 +7037,20 @@
         <v>n</v>
       </c>
       <c r="H54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J54" s="4" t="str" cm="1">
         <f t="array" ref="J54">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I54)*LEN(I54)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N54" s="4" t="str" cm="1">
         <f t="array" ref="N54">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M54)*LEN(M54)&gt;0,"")</f>
@@ -7070,7 +7070,7 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B55" s="4" t="str" cm="1">
         <f t="array" ref="B55">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A55,""),"")</f>
@@ -7085,7 +7085,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F55" s="4" t="str" cm="1">
         <f t="array" ref="F55">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E55,"")</f>
@@ -7096,20 +7096,20 @@
         <v>(%)</v>
       </c>
       <c r="H55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J55" s="4" t="str" cm="1">
         <f t="array" ref="J55">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I55)*LEN(I55)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M55" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N55" s="4" t="str" cm="1">
         <f t="array" ref="N55">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M55)*LEN(M55)&gt;0,"")</f>
@@ -7123,13 +7123,13 @@
         <v>7.1429</v>
       </c>
       <c r="U55" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="V55" s="6"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B56" s="4" t="str" cm="1">
         <f t="array" ref="B56">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A56,""),"")</f>
@@ -7144,7 +7144,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F56" s="4" t="str" cm="1">
         <f t="array" ref="F56">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E56,"")</f>
@@ -7155,20 +7155,20 @@
         <v>n</v>
       </c>
       <c r="H56" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J56" s="4" t="str" cm="1">
         <f t="array" ref="J56">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I56)*LEN(I56)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M56" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N56" s="4" t="str" cm="1">
         <f t="array" ref="N56">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M56)*LEN(M56)&gt;0,"")</f>
@@ -7188,7 +7188,7 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B57" s="4" t="str" cm="1">
         <f t="array" ref="B57">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A57,""),"")</f>
@@ -7203,7 +7203,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E57" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F57" s="4" t="str" cm="1">
         <f t="array" ref="F57">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E57,"")</f>
@@ -7214,20 +7214,20 @@
         <v>(%)</v>
       </c>
       <c r="H57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J57" s="4" t="str" cm="1">
         <f t="array" ref="J57">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I57)*LEN(I57)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N57" s="4" t="str" cm="1">
         <f t="array" ref="N57">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M57)*LEN(M57)&gt;0,"")</f>
@@ -7241,13 +7241,13 @@
         <v>92.857100000000003</v>
       </c>
       <c r="U57" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="V57" s="6"/>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B58" s="4" t="str" cm="1">
         <f t="array" ref="B58">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A58,""),"")</f>
@@ -7262,7 +7262,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E58" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F58" s="4" t="str" cm="1">
         <f t="array" ref="F58">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E58,"")</f>
@@ -7273,20 +7273,20 @@
         <v>n</v>
       </c>
       <c r="H58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J58" s="4" t="str" cm="1">
         <f t="array" ref="J58">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I58)*LEN(I58)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L58" t="s">
+        <v>230</v>
+      </c>
+      <c r="M58" t="s">
         <v>231</v>
-      </c>
-      <c r="M58" t="s">
-        <v>232</v>
       </c>
       <c r="N58" s="4" t="str" cm="1">
         <f t="array" ref="N58">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M58)*LEN(M58)&gt;0,"")</f>
@@ -7306,7 +7306,7 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B59" s="4" t="str" cm="1">
         <f t="array" ref="B59">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A59,""),"")</f>
@@ -7321,7 +7321,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F59" s="4" t="str" cm="1">
         <f t="array" ref="F59">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E59,"")</f>
@@ -7332,20 +7332,20 @@
         <v>(%)</v>
       </c>
       <c r="H59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I59" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J59" s="4" t="str" cm="1">
         <f t="array" ref="J59">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I59)*LEN(I59)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L59" t="s">
+        <v>230</v>
+      </c>
+      <c r="M59" t="s">
         <v>231</v>
-      </c>
-      <c r="M59" t="s">
-        <v>232</v>
       </c>
       <c r="N59" s="4" t="str" cm="1">
         <f t="array" ref="N59">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M59)*LEN(M59)&gt;0,"")</f>
@@ -7359,13 +7359,13 @@
         <v>1.1904999999999999</v>
       </c>
       <c r="U59" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="V59" s="6"/>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B60" s="4" t="str" cm="1">
         <f t="array" ref="B60">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A60,""),"")</f>
@@ -7380,7 +7380,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F60" s="4" t="str" cm="1">
         <f t="array" ref="F60">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E60,"")</f>
@@ -7391,20 +7391,20 @@
         <v>n</v>
       </c>
       <c r="H60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I60" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J60" s="4" t="str" cm="1">
         <f t="array" ref="J60">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I60)*LEN(I60)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N60" s="4" t="str" cm="1">
         <f t="array" ref="N60">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M60)*LEN(M60)&gt;0,"")</f>
@@ -7424,7 +7424,7 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B61" s="4" t="str" cm="1">
         <f t="array" ref="B61">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A61,""),"")</f>
@@ -7439,7 +7439,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E61" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F61" s="4" t="str" cm="1">
         <f t="array" ref="F61">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E61,"")</f>
@@ -7450,20 +7450,20 @@
         <v>(%)</v>
       </c>
       <c r="H61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I61" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J61" s="4" t="str" cm="1">
         <f t="array" ref="J61">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I61)*LEN(I61)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M61" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N61" s="4" t="str" cm="1">
         <f t="array" ref="N61">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M61)*LEN(M61)&gt;0,"")</f>
@@ -7477,13 +7477,13 @@
         <v>10.7143</v>
       </c>
       <c r="U61" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="V61" s="6"/>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B62" s="4" t="str" cm="1">
         <f t="array" ref="B62">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A62,""),"")</f>
@@ -7498,7 +7498,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E62" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F62" s="4" t="str" cm="1">
         <f t="array" ref="F62">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E62,"")</f>
@@ -7509,20 +7509,20 @@
         <v>n</v>
       </c>
       <c r="H62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J62" s="4" t="str" cm="1">
         <f t="array" ref="J62">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I62)*LEN(I62)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N62" s="4" t="str" cm="1">
         <f t="array" ref="N62">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M62)*LEN(M62)&gt;0,"")</f>
@@ -7542,7 +7542,7 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B63" s="4" t="str" cm="1">
         <f t="array" ref="B63">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A63,""),"")</f>
@@ -7557,7 +7557,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E63" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F63" s="4" t="str" cm="1">
         <f t="array" ref="F63">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E63,"")</f>
@@ -7568,20 +7568,20 @@
         <v>(%)</v>
       </c>
       <c r="H63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J63" s="4" t="str" cm="1">
         <f t="array" ref="J63">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I63)*LEN(I63)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M63" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N63" s="4" t="str" cm="1">
         <f t="array" ref="N63">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M63)*LEN(M63)&gt;0,"")</f>
@@ -7595,13 +7595,13 @@
         <v>88.095200000000006</v>
       </c>
       <c r="U63" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="V63" s="6"/>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B64" s="4" t="str" cm="1">
         <f t="array" ref="B64">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A64,""),"")</f>
@@ -7616,7 +7616,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E64" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F64" s="4" t="str" cm="1">
         <f t="array" ref="F64">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E64,"")</f>
@@ -7627,20 +7627,20 @@
         <v>n</v>
       </c>
       <c r="H64" t="s">
+        <v>223</v>
+      </c>
+      <c r="I64" t="s">
         <v>224</v>
-      </c>
-      <c r="I64" t="s">
-        <v>225</v>
       </c>
       <c r="J64" s="4" t="str" cm="1">
         <f t="array" ref="J64">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I64)*LEN(I64)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L64" t="s">
+        <v>236</v>
+      </c>
+      <c r="M64" t="s">
         <v>237</v>
-      </c>
-      <c r="M64" t="s">
-        <v>238</v>
       </c>
       <c r="N64" s="4" t="str" cm="1">
         <f t="array" ref="N64">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M64)*LEN(M64)&gt;0,"")</f>
@@ -7660,7 +7660,7 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B65" s="4" t="str" cm="1">
         <f t="array" ref="B65">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A65,""),"")</f>
@@ -7675,7 +7675,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F65" s="4" t="str" cm="1">
         <f t="array" ref="F65">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E65,"")</f>
@@ -7686,20 +7686,20 @@
         <v>(%)</v>
       </c>
       <c r="H65" t="s">
+        <v>223</v>
+      </c>
+      <c r="I65" t="s">
         <v>224</v>
-      </c>
-      <c r="I65" t="s">
-        <v>225</v>
       </c>
       <c r="J65" s="4" t="str" cm="1">
         <f t="array" ref="J65">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I65)*LEN(I65)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L65" t="s">
+        <v>236</v>
+      </c>
+      <c r="M65" t="s">
         <v>237</v>
-      </c>
-      <c r="M65" t="s">
-        <v>238</v>
       </c>
       <c r="N65" s="4" t="str" cm="1">
         <f t="array" ref="N65">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M65)*LEN(M65)&gt;0,"")</f>
@@ -7713,13 +7713,13 @@
         <v>3.4883999999999999</v>
       </c>
       <c r="U65" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="V65" s="6"/>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B66" s="4" t="str" cm="1">
         <f t="array" ref="B66">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A66,""),"")</f>
@@ -7734,7 +7734,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E66" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F66" s="4" t="str" cm="1">
         <f t="array" ref="F66">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E66,"")</f>
@@ -7745,20 +7745,20 @@
         <v>n</v>
       </c>
       <c r="H66" t="s">
+        <v>223</v>
+      </c>
+      <c r="I66" t="s">
         <v>224</v>
-      </c>
-      <c r="I66" t="s">
-        <v>225</v>
       </c>
       <c r="J66" s="4" t="str" cm="1">
         <f t="array" ref="J66">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I66)*LEN(I66)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M66" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N66" s="4" t="str" cm="1">
         <f t="array" ref="N66">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M66)*LEN(M66)&gt;0,"")</f>
@@ -7778,7 +7778,7 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B67" s="4" t="str" cm="1">
         <f t="array" ref="B67">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A67,""),"")</f>
@@ -7793,7 +7793,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E67" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F67" s="4" t="str" cm="1">
         <f t="array" ref="F67">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E67,"")</f>
@@ -7804,20 +7804,20 @@
         <v>(%)</v>
       </c>
       <c r="H67" t="s">
+        <v>223</v>
+      </c>
+      <c r="I67" t="s">
         <v>224</v>
-      </c>
-      <c r="I67" t="s">
-        <v>225</v>
       </c>
       <c r="J67" s="4" t="str" cm="1">
         <f t="array" ref="J67">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I67)*LEN(I67)&gt;0,"")</f>
         <v>Placebo</v>
       </c>
       <c r="L67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M67" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N67" s="4" t="str" cm="1">
         <f t="array" ref="N67">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M67)*LEN(M67)&gt;0,"")</f>
@@ -7831,13 +7831,13 @@
         <v>96.511600000000001</v>
       </c>
       <c r="U67" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="V67" s="6"/>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B68" s="4" t="str" cm="1">
         <f t="array" ref="B68">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A68,""),"")</f>
@@ -7852,7 +7852,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F68" s="4" t="str" cm="1">
         <f t="array" ref="F68">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E68,"")</f>
@@ -7863,20 +7863,20 @@
         <v>n</v>
       </c>
       <c r="H68" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J68" s="4" t="str" cm="1">
         <f t="array" ref="J68">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I68)*LEN(I68)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L68" t="s">
+        <v>236</v>
+      </c>
+      <c r="M68" t="s">
         <v>237</v>
-      </c>
-      <c r="M68" t="s">
-        <v>238</v>
       </c>
       <c r="N68" s="4" t="str" cm="1">
         <f t="array" ref="N68">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M68)*LEN(M68)&gt;0,"")</f>
@@ -7896,7 +7896,7 @@
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B69" s="4" t="str" cm="1">
         <f t="array" ref="B69">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A69,""),"")</f>
@@ -7911,7 +7911,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E69" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F69" s="4" t="str" cm="1">
         <f t="array" ref="F69">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E69,"")</f>
@@ -7922,20 +7922,20 @@
         <v>(%)</v>
       </c>
       <c r="H69" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J69" s="4" t="str" cm="1">
         <f t="array" ref="J69">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I69)*LEN(I69)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L69" t="s">
+        <v>236</v>
+      </c>
+      <c r="M69" t="s">
         <v>237</v>
-      </c>
-      <c r="M69" t="s">
-        <v>238</v>
       </c>
       <c r="N69" s="4" t="str" cm="1">
         <f t="array" ref="N69">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M69)*LEN(M69)&gt;0,"")</f>
@@ -7949,13 +7949,13 @@
         <v>7.1429</v>
       </c>
       <c r="U69" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="V69" s="6"/>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B70" s="4" t="str" cm="1">
         <f t="array" ref="B70">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A70,""),"")</f>
@@ -7970,7 +7970,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E70" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F70" s="4" t="str" cm="1">
         <f t="array" ref="F70">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E70,"")</f>
@@ -7981,20 +7981,20 @@
         <v>n</v>
       </c>
       <c r="H70" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J70" s="4" t="str" cm="1">
         <f t="array" ref="J70">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I70)*LEN(I70)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L70" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M70" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N70" s="4" t="str" cm="1">
         <f t="array" ref="N70">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M70)*LEN(M70)&gt;0,"")</f>
@@ -8014,7 +8014,7 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B71" s="4" t="str" cm="1">
         <f t="array" ref="B71">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A71,""),"")</f>
@@ -8029,7 +8029,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F71" s="4" t="str" cm="1">
         <f t="array" ref="F71">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E71,"")</f>
@@ -8040,20 +8040,20 @@
         <v>(%)</v>
       </c>
       <c r="H71" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J71" s="4" t="str" cm="1">
         <f t="array" ref="J71">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I71)*LEN(I71)&gt;0,"")</f>
         <v>Xanomeline Low Dose</v>
       </c>
       <c r="L71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N71" s="4" t="str" cm="1">
         <f t="array" ref="N71">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M71)*LEN(M71)&gt;0,"")</f>
@@ -8067,13 +8067,13 @@
         <v>92.857100000000003</v>
       </c>
       <c r="U71" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="V71" s="6"/>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B72" s="4" t="str" cm="1">
         <f t="array" ref="B72">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A72,""),"")</f>
@@ -8088,7 +8088,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F72" s="4" t="str" cm="1">
         <f t="array" ref="F72">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E72,"")</f>
@@ -8099,20 +8099,20 @@
         <v>n</v>
       </c>
       <c r="H72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J72" s="4" t="str" cm="1">
         <f t="array" ref="J72">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I72)*LEN(I72)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L72" t="s">
+        <v>236</v>
+      </c>
+      <c r="M72" t="s">
         <v>237</v>
-      </c>
-      <c r="M72" t="s">
-        <v>238</v>
       </c>
       <c r="N72" s="4" t="str" cm="1">
         <f t="array" ref="N72">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M72)*LEN(M72)&gt;0,"")</f>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B73" s="4" t="str" cm="1">
         <f t="array" ref="B73">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A73,""),"")</f>
@@ -8147,7 +8147,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E73" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F73" s="4" t="str" cm="1">
         <f t="array" ref="F73">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E73,"")</f>
@@ -8158,20 +8158,20 @@
         <v>(%)</v>
       </c>
       <c r="H73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I73" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J73" s="4" t="str" cm="1">
         <f t="array" ref="J73">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I73)*LEN(I73)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L73" t="s">
+        <v>236</v>
+      </c>
+      <c r="M73" t="s">
         <v>237</v>
-      </c>
-      <c r="M73" t="s">
-        <v>238</v>
       </c>
       <c r="N73" s="4" t="str" cm="1">
         <f t="array" ref="N73">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M73)*LEN(M73)&gt;0,"")</f>
@@ -8185,13 +8185,13 @@
         <v>3.5714000000000001</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="V73" s="6"/>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B74" s="4" t="str" cm="1">
         <f t="array" ref="B74">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A74,""),"")</f>
@@ -8206,7 +8206,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F74" s="4" t="str" cm="1">
         <f t="array" ref="F74">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E74,"")</f>
@@ -8217,20 +8217,20 @@
         <v>n</v>
       </c>
       <c r="H74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I74" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J74" s="4" t="str" cm="1">
         <f t="array" ref="J74">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I74)*LEN(I74)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N74" s="4" t="str" cm="1">
         <f t="array" ref="N74">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M74)*LEN(M74)&gt;0,"")</f>
@@ -8250,7 +8250,7 @@
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B75" s="4" t="str" cm="1">
         <f t="array" ref="B75">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A75,""),"")</f>
@@ -8265,7 +8265,7 @@
         <v>Grouped summary of categorical variable</v>
       </c>
       <c r="E75" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F75" s="4" t="str" cm="1">
         <f t="array" ref="F75">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$27,AnalysisMethods!$E$2:$E$27=AnalysisResults!E75,"")</f>
@@ -8276,20 +8276,20 @@
         <v>(%)</v>
       </c>
       <c r="H75" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J75" s="4" t="str" cm="1">
         <f t="array" ref="J75">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!I75)*LEN(I75)&gt;0,"")</f>
         <v>Xanomeline High Dose</v>
       </c>
       <c r="L75" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N75" s="4" t="str" cm="1">
         <f t="array" ref="N75">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$18,(AnalysisGroupings!$F$2:$F$18=AnalysisResults!M75)*LEN(M75)&gt;0,"")</f>
@@ -8303,7 +8303,7 @@
         <v>96.428600000000003</v>
       </c>
       <c r="U75" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="V75" s="6"/>
     </row>
@@ -8445,7 +8445,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -8459,7 +8459,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -8484,7 +8484,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -8509,7 +8509,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -8534,7 +8534,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -8559,7 +8559,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -8584,7 +8584,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -8634,7 +8634,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -8730,7 +8730,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -8740,10 +8740,10 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>88</v>
@@ -8804,7 +8804,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
         <v>206</v>
@@ -8822,7 +8822,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H2" t="s">
         <v>201</v>
@@ -8830,7 +8830,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B3" t="s">
         <v>206</v>
@@ -8848,7 +8848,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H3" t="s">
         <v>90</v>
@@ -8856,7 +8856,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
         <v>206</v>
@@ -8874,7 +8874,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H4" t="s">
         <v>202</v>
@@ -8882,7 +8882,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
         <v>206</v>
@@ -8900,7 +8900,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H5" t="s">
         <v>203</v>
@@ -8908,7 +8908,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B6" t="s">
         <v>206</v>
@@ -8926,7 +8926,7 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H6" t="s">
         <v>204</v>
@@ -8934,7 +8934,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s">
         <v>206</v>
@@ -8952,7 +8952,7 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H7" t="s">
         <v>205</v>
@@ -8995,13 +8995,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>